<commit_message>
0.9.0 version of hoemyavr
</commit_message>
<xml_diff>
--- a/src/gen/avrcodes.xlsx
+++ b/src/gen/avrcodes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="319">
   <si>
     <t>group</t>
   </si>
@@ -166,6 +166,9 @@
     <t>ZMON</t>
   </si>
   <si>
+    <t>mzpower_on</t>
+  </si>
+  <si>
     <t>mzpower.on</t>
   </si>
   <si>
@@ -175,6 +178,9 @@
     <t>ZMOFF</t>
   </si>
   <si>
+    <t>mzpower_off</t>
+  </si>
+  <si>
     <t>mzpower.off</t>
   </si>
   <si>
@@ -182,6 +188,9 @@
   </si>
   <si>
     <t>ZM?</t>
+  </si>
+  <si>
+    <t>mzpower_request</t>
   </si>
   <si>
     <t>mzpower.request</t>
@@ -1389,18 +1398,17 @@
   </sheetPr>
   <dimension ref="A1:AG72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="45" min="6" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="46" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="45" min="6" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,13 +1821,13 @@
         <v>47</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>38</v>
@@ -1911,16 +1919,16 @@
         <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>38</v>
@@ -2012,13 +2020,13 @@
         <v>46</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="s">
@@ -2108,19 +2116,19 @@
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>38</v>
@@ -2209,19 +2217,19 @@
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>38</v>
@@ -2310,19 +2318,19 @@
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>38</v>
@@ -2411,16 +2419,16 @@
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="6" t="s">
@@ -2510,19 +2518,19 @@
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>38</v>
@@ -2611,19 +2619,19 @@
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>38</v>
@@ -2712,16 +2720,16 @@
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
@@ -2811,19 +2819,19 @@
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>38</v>
@@ -2871,60 +2879,60 @@
         <v>38</v>
       </c>
       <c r="U15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG15" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>38</v>
@@ -3013,19 +3021,19 @@
     </row>
     <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>38</v>
@@ -3106,27 +3114,27 @@
         <v>38</v>
       </c>
       <c r="AF17" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG17" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>38</v>
@@ -3215,19 +3223,19 @@
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>38</v>
@@ -3316,19 +3324,19 @@
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>38</v>
@@ -3373,7 +3381,7 @@
         <v>38</v>
       </c>
       <c r="T20" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U20" s="6" t="s">
         <v>38</v>
@@ -3391,7 +3399,7 @@
         <v>38</v>
       </c>
       <c r="Z20" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA20" s="6" t="s">
         <v>38</v>
@@ -3406,7 +3414,7 @@
         <v>38</v>
       </c>
       <c r="AE20" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF20" s="6" t="s">
         <v>38</v>
@@ -3417,120 +3425,120 @@
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T21" s="6" t="s">
         <v>38</v>
       </c>
       <c r="U21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z21" s="6" t="s">
         <v>38</v>
       </c>
       <c r="AA21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE21" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AF21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG21" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>38</v>
@@ -3545,7 +3553,7 @@
         <v>38</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>38</v>
@@ -3560,7 +3568,7 @@
         <v>38</v>
       </c>
       <c r="O22" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>38</v>
@@ -3575,10 +3583,10 @@
         <v>38</v>
       </c>
       <c r="T22" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U22" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V22" s="6" t="s">
         <v>38</v>
@@ -3593,7 +3601,7 @@
         <v>38</v>
       </c>
       <c r="Z22" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA22" s="6" t="s">
         <v>38</v>
@@ -3608,7 +3616,7 @@
         <v>38</v>
       </c>
       <c r="AE22" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF22" s="6" t="s">
         <v>38</v>
@@ -3619,61 +3627,61 @@
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T23" s="6" t="s">
         <v>38</v>
@@ -3682,57 +3690,57 @@
         <v>38</v>
       </c>
       <c r="V23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z23" s="6" t="s">
         <v>38</v>
       </c>
       <c r="AA23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG23" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>38</v>
@@ -3821,120 +3829,120 @@
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O25" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U25" s="6" t="s">
         <v>38</v>
       </c>
       <c r="V25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z25" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG25" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>38</v>
@@ -4023,40 +4031,40 @@
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>38</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>38</v>
@@ -4068,10 +4076,10 @@
         <v>38</v>
       </c>
       <c r="P27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R27" s="6" t="s">
         <v>38</v>
@@ -4080,16 +4088,16 @@
         <v>38</v>
       </c>
       <c r="T27" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U27" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X27" s="6" t="s">
         <v>38</v>
@@ -4098,13 +4106,13 @@
         <v>38</v>
       </c>
       <c r="Z27" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB27" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC27" s="6" t="s">
         <v>38</v>
@@ -4113,7 +4121,7 @@
         <v>38</v>
       </c>
       <c r="AE27" s="18" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF27" s="6" t="s">
         <v>38</v>
@@ -4124,120 +4132,120 @@
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="U28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="AA28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE28" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AF28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG28" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>38</v>
@@ -4255,7 +4263,7 @@
         <v>38</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>38</v>
@@ -4270,7 +4278,7 @@
         <v>38</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>38</v>
@@ -4285,10 +4293,10 @@
         <v>38</v>
       </c>
       <c r="U29" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V29" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W29" s="6" t="s">
         <v>38</v>
@@ -4303,7 +4311,7 @@
         <v>38</v>
       </c>
       <c r="AA29" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB29" s="7" t="s">
         <v>38</v>
@@ -4318,7 +4326,7 @@
         <v>38</v>
       </c>
       <c r="AF29" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG29" s="7" t="s">
         <v>38</v>
@@ -4326,19 +4334,19 @@
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>38</v>
@@ -4386,7 +4394,7 @@
         <v>38</v>
       </c>
       <c r="U30" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V30" s="6" t="s">
         <v>38</v>
@@ -4427,19 +4435,19 @@
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>38</v>
@@ -4487,7 +4495,7 @@
         <v>38</v>
       </c>
       <c r="U31" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V31" s="6" t="s">
         <v>38</v>
@@ -4528,19 +4536,19 @@
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>38</v>
@@ -4588,7 +4596,7 @@
         <v>38</v>
       </c>
       <c r="U32" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V32" s="6" t="s">
         <v>38</v>
@@ -4629,73 +4637,73 @@
     </row>
     <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O33" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W33" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X33" s="6" t="s">
         <v>38</v>
@@ -4707,42 +4715,42 @@
         <v>38</v>
       </c>
       <c r="AA33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG33" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>38</v>
@@ -4757,7 +4765,7 @@
         <v>38</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>38</v>
@@ -4772,7 +4780,7 @@
         <v>38</v>
       </c>
       <c r="O34" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P34" s="6" t="s">
         <v>38</v>
@@ -4790,7 +4798,7 @@
         <v>38</v>
       </c>
       <c r="U34" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V34" s="6" t="s">
         <v>38</v>
@@ -4820,7 +4828,7 @@
         <v>38</v>
       </c>
       <c r="AE34" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF34" s="7" t="s">
         <v>38</v>
@@ -4831,19 +4839,19 @@
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>38</v>
@@ -4858,7 +4866,7 @@
         <v>38</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>38</v>
@@ -4873,7 +4881,7 @@
         <v>38</v>
       </c>
       <c r="O35" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>38</v>
@@ -4891,7 +4899,7 @@
         <v>38</v>
       </c>
       <c r="U35" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V35" s="6" t="s">
         <v>38</v>
@@ -4903,10 +4911,10 @@
         <v>38</v>
       </c>
       <c r="Y35" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z35" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA35" s="6" t="s">
         <v>38</v>
@@ -4918,33 +4926,33 @@
         <v>38</v>
       </c>
       <c r="AD35" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE35" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF35" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG35" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>38</v>
@@ -4953,99 +4961,99 @@
         <v>38</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG36" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>38</v>
@@ -5054,99 +5062,99 @@
         <v>38</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG37" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>38</v>
@@ -5155,99 +5163,99 @@
         <v>38</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG38" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>38</v>
@@ -5256,99 +5264,99 @@
         <v>38</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG39" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>38</v>
@@ -5357,99 +5365,99 @@
         <v>38</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG40" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>38</v>
@@ -5464,7 +5472,7 @@
         <v>38</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K41" s="6" t="s">
         <v>38</v>
@@ -5494,10 +5502,10 @@
         <v>38</v>
       </c>
       <c r="T41" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U41" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V41" s="6" t="s">
         <v>38</v>
@@ -5512,7 +5520,7 @@
         <v>38</v>
       </c>
       <c r="Z41" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA41" s="6" t="s">
         <v>38</v>
@@ -5527,7 +5535,7 @@
         <v>38</v>
       </c>
       <c r="AE41" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF41" s="6" t="s">
         <v>38</v>
@@ -5538,135 +5546,135 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O42" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T42" s="6" t="s">
         <v>38</v>
       </c>
       <c r="U42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z42" s="6" t="s">
         <v>38</v>
       </c>
       <c r="AA42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE42" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AF42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG42" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>38</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>38</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>38</v>
@@ -5675,13 +5683,13 @@
         <v>38</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P43" s="6" t="s">
         <v>38</v>
@@ -5690,16 +5698,16 @@
         <v>38</v>
       </c>
       <c r="R43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V43" s="6" t="s">
         <v>38</v>
@@ -5708,13 +5716,13 @@
         <v>38</v>
       </c>
       <c r="X43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA43" s="6" t="s">
         <v>38</v>
@@ -5723,45 +5731,45 @@
         <v>38</v>
       </c>
       <c r="AC43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF43" s="22" t="s">
         <v>38</v>
       </c>
       <c r="AG43" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>38</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>38</v>
@@ -5770,10 +5778,10 @@
         <v>38</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>38</v>
@@ -5785,10 +5793,10 @@
         <v>38</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R44" s="6" t="s">
         <v>38</v>
@@ -5803,10 +5811,10 @@
         <v>38</v>
       </c>
       <c r="V44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X44" s="6" t="s">
         <v>38</v>
@@ -5818,10 +5826,10 @@
         <v>38</v>
       </c>
       <c r="AA44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB44" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC44" s="7" t="s">
         <v>38</v>
@@ -5833,7 +5841,7 @@
         <v>38</v>
       </c>
       <c r="AF44" s="19" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG44" s="7" t="s">
         <v>38</v>
@@ -5841,19 +5849,19 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>38</v>
@@ -5942,19 +5950,19 @@
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>38</v>
@@ -6043,19 +6051,19 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>38</v>
@@ -6144,19 +6152,19 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>38</v>
@@ -6171,7 +6179,7 @@
         <v>38</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K48" s="6" t="s">
         <v>38</v>
@@ -6186,7 +6194,7 @@
         <v>38</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P48" s="6" t="s">
         <v>38</v>
@@ -6204,7 +6212,7 @@
         <v>38</v>
       </c>
       <c r="U48" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V48" s="6" t="s">
         <v>38</v>
@@ -6245,19 +6253,19 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>38</v>
@@ -6272,7 +6280,7 @@
         <v>38</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>38</v>
@@ -6287,7 +6295,7 @@
         <v>38</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P49" s="6" t="s">
         <v>38</v>
@@ -6305,7 +6313,7 @@
         <v>38</v>
       </c>
       <c r="U49" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V49" s="6" t="s">
         <v>38</v>
@@ -6346,117 +6354,117 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T50" s="6" t="s">
         <v>38</v>
       </c>
       <c r="U50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z50" s="6" t="s">
         <v>38</v>
       </c>
       <c r="AA50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE50" s="7" t="s">
         <v>38</v>
       </c>
       <c r="AF50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG50" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="E51" s="21"/>
       <c r="F51" s="6" t="s">
@@ -6546,34 +6554,34 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>38</v>
@@ -6582,13 +6590,13 @@
         <v>38</v>
       </c>
       <c r="M52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P52" s="6" t="s">
         <v>38</v>
@@ -6597,16 +6605,16 @@
         <v>38</v>
       </c>
       <c r="R52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V52" s="6" t="s">
         <v>38</v>
@@ -6615,13 +6623,13 @@
         <v>38</v>
       </c>
       <c r="X52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA52" s="6" t="s">
         <v>38</v>
@@ -6630,51 +6638,51 @@
         <v>38</v>
       </c>
       <c r="AC52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF52" s="22" t="s">
         <v>38</v>
       </c>
       <c r="AG52" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>38</v>
@@ -6683,13 +6691,13 @@
         <v>38</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P53" s="6" t="s">
         <v>38</v>
@@ -6698,16 +6706,16 @@
         <v>38</v>
       </c>
       <c r="R53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V53" s="6" t="s">
         <v>38</v>
@@ -6716,13 +6724,13 @@
         <v>38</v>
       </c>
       <c r="X53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA53" s="6" t="s">
         <v>38</v>
@@ -6731,51 +6739,51 @@
         <v>38</v>
       </c>
       <c r="AC53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF53" s="22" t="s">
         <v>38</v>
       </c>
       <c r="AG53" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>38</v>
@@ -6784,13 +6792,13 @@
         <v>38</v>
       </c>
       <c r="M54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P54" s="6" t="s">
         <v>38</v>
@@ -6799,16 +6807,16 @@
         <v>38</v>
       </c>
       <c r="R54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V54" s="6" t="s">
         <v>38</v>
@@ -6817,13 +6825,13 @@
         <v>38</v>
       </c>
       <c r="X54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA54" s="6" t="s">
         <v>38</v>
@@ -6832,49 +6840,49 @@
         <v>38</v>
       </c>
       <c r="AC54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF54" s="22" t="s">
         <v>38</v>
       </c>
       <c r="AG54" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>38</v>
@@ -6883,13 +6891,13 @@
         <v>38</v>
       </c>
       <c r="M55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P55" s="6" t="s">
         <v>38</v>
@@ -6898,16 +6906,16 @@
         <v>38</v>
       </c>
       <c r="R55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V55" s="6" t="s">
         <v>38</v>
@@ -6916,13 +6924,13 @@
         <v>38</v>
       </c>
       <c r="X55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA55" s="6" t="s">
         <v>38</v>
@@ -6931,36 +6939,36 @@
         <v>38</v>
       </c>
       <c r="AC55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF55" s="22" t="s">
         <v>38</v>
       </c>
       <c r="AG55" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>38</v>
@@ -6975,7 +6983,7 @@
         <v>38</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>38</v>
@@ -6990,7 +6998,7 @@
         <v>38</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>38</v>
@@ -7005,10 +7013,10 @@
         <v>38</v>
       </c>
       <c r="T56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V56" s="6" t="s">
         <v>38</v>
@@ -7023,7 +7031,7 @@
         <v>38</v>
       </c>
       <c r="Z56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA56" s="6" t="s">
         <v>38</v>
@@ -7038,7 +7046,7 @@
         <v>38</v>
       </c>
       <c r="AE56" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF56" s="6" t="s">
         <v>38</v>
@@ -7049,19 +7057,19 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>38</v>
@@ -7076,7 +7084,7 @@
         <v>38</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>38</v>
@@ -7091,7 +7099,7 @@
         <v>38</v>
       </c>
       <c r="O57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>38</v>
@@ -7106,10 +7114,10 @@
         <v>38</v>
       </c>
       <c r="T57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V57" s="6" t="s">
         <v>38</v>
@@ -7124,7 +7132,7 @@
         <v>38</v>
       </c>
       <c r="Z57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA57" s="6" t="s">
         <v>38</v>
@@ -7139,7 +7147,7 @@
         <v>38</v>
       </c>
       <c r="AE57" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF57" s="6" t="s">
         <v>38</v>
@@ -7150,19 +7158,19 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>38</v>
@@ -7177,7 +7185,7 @@
         <v>38</v>
       </c>
       <c r="J58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K58" s="6" t="s">
         <v>38</v>
@@ -7192,7 +7200,7 @@
         <v>38</v>
       </c>
       <c r="O58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>38</v>
@@ -7207,10 +7215,10 @@
         <v>38</v>
       </c>
       <c r="T58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V58" s="6" t="s">
         <v>38</v>
@@ -7225,7 +7233,7 @@
         <v>38</v>
       </c>
       <c r="Z58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA58" s="6" t="s">
         <v>38</v>
@@ -7240,7 +7248,7 @@
         <v>38</v>
       </c>
       <c r="AE58" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF58" s="6" t="s">
         <v>38</v>
@@ -7251,19 +7259,19 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>38</v>
@@ -7352,19 +7360,19 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>38</v>
@@ -7453,19 +7461,19 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>38</v>
@@ -7554,19 +7562,19 @@
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>38</v>
@@ -7655,221 +7663,221 @@
     </row>
     <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J63" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O63" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U63" s="6" t="s">
         <v>38</v>
       </c>
       <c r="V63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z63" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG63" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O64" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U64" s="6" t="s">
         <v>38</v>
       </c>
       <c r="V64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z64" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG64" s="14" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E65" s="24" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>38</v>
@@ -7958,19 +7966,19 @@
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C66" s="24" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E66" s="24" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>38</v>
@@ -8059,19 +8067,19 @@
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>38</v>
@@ -8160,120 +8168,120 @@
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>38</v>
       </c>
       <c r="K68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="L68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O68" s="6" t="s">
         <v>38</v>
       </c>
       <c r="P68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="S68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="T68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="U68" s="6" t="s">
         <v>38</v>
       </c>
       <c r="V68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="W68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="X68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Y68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AB68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AC68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AD68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AE68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AG68" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>38</v>
@@ -8362,19 +8370,19 @@
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>38</v>
@@ -8389,7 +8397,7 @@
         <v>38</v>
       </c>
       <c r="J70" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>38</v>
@@ -8404,7 +8412,7 @@
         <v>38</v>
       </c>
       <c r="O70" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P70" s="6" t="s">
         <v>38</v>
@@ -8422,7 +8430,7 @@
         <v>38</v>
       </c>
       <c r="U70" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V70" s="6" t="s">
         <v>38</v>
@@ -8463,19 +8471,19 @@
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>38</v>
@@ -8490,7 +8498,7 @@
         <v>38</v>
       </c>
       <c r="J71" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>38</v>
@@ -8505,7 +8513,7 @@
         <v>38</v>
       </c>
       <c r="O71" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P71" s="6" t="s">
         <v>38</v>
@@ -8523,7 +8531,7 @@
         <v>38</v>
       </c>
       <c r="U71" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="V71" s="6" t="s">
         <v>38</v>
@@ -8564,16 +8572,16 @@
     </row>
     <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="6" t="s">
@@ -8637,7 +8645,7 @@
         <v>38</v>
       </c>
       <c r="Z72" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA72" s="6" t="s">
         <v>38</v>
@@ -8652,7 +8660,7 @@
         <v>38</v>
       </c>
       <c r="AE72" s="13" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AF72" s="6" t="s">
         <v>38</v>

</xml_diff>